<commit_message>
Reference lists and functions modifications
</commit_message>
<xml_diff>
--- a/Metiers/Reference_lists/Code-ERSGearType-v1.1.xlsx
+++ b/Metiers/Reference_lists/Code-ERSGearType-v1.1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\joeg\Metier work\RCG_intersessional_work_2021\Meeting 210325\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madamowicz\Documents\Dokumenty\GitHub\RCGs\Metiers\Reference_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28005" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13440" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="formatted" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">formatted!$A$1:$F$67</definedName>
     <definedName name="OLE_LINK7" localSheetId="1">formatted!#REF!</definedName>
     <definedName name="OLE_LINK7" localSheetId="0">Sheet1!$B$6</definedName>
   </definedNames>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="189">
   <si>
     <t>Code</t>
   </si>
@@ -557,13 +558,40 @@
     <t>Transcribing agreed ?</t>
   </si>
   <si>
+    <t>Adding metier "GNC_DEF_&gt;0_0_0" ?</t>
+  </si>
+  <si>
+    <t>Adding metier "SPR_DEF_&gt;0_0_0" ?</t>
+  </si>
+  <si>
     <t>Gear transcoding</t>
   </si>
   <si>
     <t>Transcoding proposal</t>
   </si>
   <si>
-    <t>GEAR_Level6</t>
+    <t>GEAR Level6</t>
+  </si>
+  <si>
+    <t>DWS</t>
+  </si>
+  <si>
+    <t>To be validated</t>
+  </si>
+  <si>
+    <t>Adding metier LA_SPF_&gt;0_0_0 &amp; LA_LPF_&gt;0_0_0 ?</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>LDF,NSEA,Natl,MED,BALT</t>
+  </si>
+  <si>
+    <t>DWS_for_RCG</t>
   </si>
 </sst>
 </file>
@@ -670,7 +698,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -694,12 +722,320 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -710,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -758,141 +1094,361 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -908,9 +1464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -948,7 +1504,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1020,7 +1576,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1674,1116 +2230,1456 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="18"/>
-    <col min="8" max="8" width="39.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="17"/>
+    <col min="10" max="10" width="39.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="44" t="s">
         <v>89</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="F1" s="130" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="E2" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+      <c r="E3" s="66"/>
+      <c r="F3" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" s="70"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="52" t="s">
+      <c r="E4" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="84"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="134" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="135" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="68" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="38" t="s">
+      <c r="F9" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="70"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="66"/>
+      <c r="F10" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="70"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="66"/>
+      <c r="F11" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="98"/>
+      <c r="F13" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="84"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="101" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="103"/>
+      <c r="F14" s="134" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="91"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="105" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="106" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="107" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="108"/>
+      <c r="F15" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="71"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="98"/>
+      <c r="F16" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="84"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="110" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="108"/>
+      <c r="F17" s="131" t="s">
+        <v>186</v>
+      </c>
+      <c r="G17" s="71" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="66"/>
+      <c r="F18" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="66"/>
+      <c r="F19" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G20" s="72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="66"/>
+      <c r="F21" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="66"/>
+      <c r="F23" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="66"/>
+      <c r="F24" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G24" s="70"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F25" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="111" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="112" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="113" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="137" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="108"/>
+      <c r="F28" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="71"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G29" s="70"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="70"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="114" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="115" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G31" s="84"/>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="52" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="56" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="61"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="44"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="44"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="44"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="44"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="44"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="44"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="44"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="44"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="44"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="44"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="44"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="44"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="44"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
+      <c r="B32" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="30" t="s">
+      <c r="E32" s="103"/>
+      <c r="F32" s="134" t="s">
+        <v>186</v>
+      </c>
+      <c r="G32" s="91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="117" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="120" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="44"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="59"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="41" t="s">
+      <c r="E33" s="121" t="s">
+        <v>183</v>
+      </c>
+      <c r="F33" s="134" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" s="91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="44"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
+      <c r="E34" s="108"/>
+      <c r="F34" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" s="71"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+      <c r="E35" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F35" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G35" s="70"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="44"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="41" t="s">
+      <c r="E36" s="66"/>
+      <c r="F36" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="70"/>
+    </row>
+    <row r="37" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="114" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="41" t="s">
+      <c r="E37" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="F37" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="84"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="44"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
+      <c r="E38" s="108"/>
+      <c r="F38" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="71"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="44"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="20" t="s">
+      <c r="E39" s="66"/>
+      <c r="F39" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G39" s="70"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="48" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="61"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
+      <c r="E40" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="70"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="44"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="20" t="s">
+      <c r="E41" s="66"/>
+      <c r="F41" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G41" s="70"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="44"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
+      <c r="E42" s="66"/>
+      <c r="F42" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G42" s="70"/>
+    </row>
+    <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="69" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
+      <c r="F43" s="137" t="s">
+        <v>185</v>
+      </c>
+      <c r="G43" s="73"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="62"/>
-      <c r="E44" s="61"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
+      <c r="D44" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="123" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G44" s="71"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="44"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
+      <c r="E45" s="66"/>
+      <c r="F45" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G45" s="70"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="32" t="s">
+      <c r="D46" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="E46" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G46" s="70"/>
+    </row>
+    <row r="47" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="20" t="s">
+      <c r="E47" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="F47" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G47" s="84"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="31" t="s">
+      <c r="D48" s="127" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E48" s="128" t="s">
+        <v>180</v>
+      </c>
+      <c r="F48" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="G48" s="71"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="59" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="50" t="s">
+      <c r="F49" s="136" t="s">
+        <v>185</v>
+      </c>
+      <c r="G49" s="72"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="41" t="s">
+      <c r="D50" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="36" t="s">
+      <c r="E50" s="66"/>
+      <c r="F50" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G50" s="70"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" s="44"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="20" t="s">
+      <c r="D51" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="24" t="s">
+      <c r="E51" s="66"/>
+      <c r="F51" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G51" s="70"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" s="44"/>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="41" t="s">
+      <c r="D52" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="36" t="s">
+      <c r="E52" s="66"/>
+      <c r="F52" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G52" s="70"/>
+    </row>
+    <row r="53" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E52" s="44"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="41" t="s">
+      <c r="D53" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53" s="44"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="41" t="s">
+      <c r="E53" s="98"/>
+      <c r="F53" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="84"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="47" t="s">
+      <c r="C54" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="46" t="s">
+      <c r="D54" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="56" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
+      <c r="F54" s="138" t="s">
+        <v>186</v>
+      </c>
+      <c r="G54" s="85" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="30" t="s">
+      <c r="D55" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E55" s="44"/>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
+      <c r="E55" s="66"/>
+      <c r="F55" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G55" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="E56" s="44"/>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
+      <c r="E56" s="66"/>
+      <c r="F56" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G56" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="44"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="s">
+      <c r="E57" s="66"/>
+      <c r="F57" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="44"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="s">
+      <c r="E58" s="66"/>
+      <c r="F58" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G58" s="70"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="44"/>
-    </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="20" t="s">
+      <c r="E59" s="66"/>
+      <c r="F59" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G59" s="70"/>
+    </row>
+    <row r="60" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="F60"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-    </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="20" t="s">
+      <c r="F60" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G60" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="H60"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+    </row>
+    <row r="61" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="44"/>
-      <c r="F61"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-    </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="20" t="s">
+      <c r="E61" s="66"/>
+      <c r="F61" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="G61" s="70"/>
+      <c r="H61"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+    </row>
+    <row r="62" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="32" t="s">
+      <c r="D62" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E62" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="F62"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-    </row>
-    <row r="63" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="20" t="s">
+      <c r="E62" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F62" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G62" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="H62"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+    </row>
+    <row r="63" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E63" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="F63"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="41" t="s">
+      <c r="E63" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G63" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="H63"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C64" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D64" s="32" t="s">
+      <c r="D64" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E64" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="48" t="s">
+      <c r="E64" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F64" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="G64" s="70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="48" t="s">
+      <c r="B65" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C65" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="31" t="s">
+      <c r="D65" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="E65" s="59" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="41" t="s">
+      <c r="F65" s="136" t="s">
+        <v>186</v>
+      </c>
+      <c r="G65" s="72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="47" t="s">
+      <c r="C66" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="46" t="s">
+      <c r="D66" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="E66" s="31" t="s">
+      <c r="E66" s="59" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
+      <c r="F66" s="136" t="s">
+        <v>185</v>
+      </c>
+      <c r="G66" s="72"/>
+    </row>
+    <row r="67" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="C67" s="47" t="s">
+      <c r="C67" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="46" t="s">
+      <c r="D67" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="E67" s="31" t="s">
+      <c r="E67" s="69" t="s">
         <v>168</v>
+      </c>
+      <c r="F67" s="137" t="s">
+        <v>186</v>
+      </c>
+      <c r="G67" s="73" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>